<commit_message>
uploaded correct todo list
uploaded newer copy
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="20">
   <si>
     <t>Task Description</t>
   </si>
@@ -68,13 +68,22 @@
     <t>bugchecking/fixing</t>
   </si>
   <si>
-    <t>all</t>
-  </si>
-  <si>
     <t>finishing touches + testing + extra features</t>
   </si>
   <si>
     <t>total</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>CSS</t>
+  </si>
+  <si>
+    <t>HTML</t>
+  </si>
+  <si>
+    <t>JavaScript</t>
   </si>
 </sst>
 </file>
@@ -395,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -409,7 +418,7 @@
     <col min="4" max="4" width="13.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -422,8 +431,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -431,10 +443,13 @@
         <v>0.5</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -442,10 +457,13 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -455,8 +473,11 @@
       <c r="C4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -466,8 +487,11 @@
       <c r="C5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -475,10 +499,13 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -486,10 +513,13 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -497,24 +527,257 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>0.5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23">
+        <v>3</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
         <v>15</v>
       </c>
-      <c r="B9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11">
-        <f>SUM(B2:B10)</f>
-        <v>15.5</v>
+      <c r="B27">
+        <f>SUM(B2:B26)</f>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>